<commit_message>
Updated Documentation and added presentation (Unfinished)
</commit_message>
<xml_diff>
--- a/Documentation/Risk Assessment.xlsx
+++ b/Documentation/Risk Assessment.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\QA\Desktop\IMS\IMS-22EnableMay2\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\QA\Desktop\FootballTeamGenerator\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E5E0176-E36C-4156-BEE0-ABC736EB7789}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAB9C36C-2E82-42FA-9DD7-A30AFBDCEF7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{7FDBD9BC-9C30-4BBF-83F1-F1573D2F17F5}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="59">
   <si>
     <t>Description</t>
   </si>
@@ -200,6 +200,18 @@
   </si>
   <si>
     <t>Keep Local copy of files.</t>
+  </si>
+  <si>
+    <t>Web Server goes down</t>
+  </si>
+  <si>
+    <t>If deployed, then website becomes unaccessible</t>
+  </si>
+  <si>
+    <t>Hosting Service</t>
+  </si>
+  <si>
+    <t>None</t>
   </si>
 </sst>
 </file>
@@ -243,7 +255,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -307,6 +319,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC65911"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -362,7 +392,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -414,32 +444,24 @@
     <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="3" fillId="13" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="14" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="12" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="3">
     <dxf>
       <fill>
         <patternFill>
@@ -457,7 +479,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="7"/>
+          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -779,10 +801,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C87F0CF8-F88A-4D21-ACF1-D6F81608C049}">
-  <dimension ref="A1:Q19"/>
+  <dimension ref="A1:Q20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -829,93 +851,90 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="42.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="13" t="s">
+    <row r="2" spans="1:17" s="24" customFormat="1" ht="23.25" x14ac:dyDescent="0.45">
+      <c r="A2" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="F2" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="G2" s="23"/>
+      <c r="H2" s="27" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" ht="42.4" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A3" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B3" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" s="13"/>
-      <c r="H2" s="15" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" ht="40.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="13" t="s">
-        <v>14</v>
-      </c>
       <c r="C3" s="14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E3" s="13" t="s">
         <v>11</v>
       </c>
       <c r="F3" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="G3" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="H3" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q3" s="2"/>
-    </row>
-    <row r="4" spans="1:17" ht="46.5" x14ac:dyDescent="0.45">
+        <v>12</v>
+      </c>
+      <c r="G3" s="13"/>
+      <c r="H3" s="15" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" ht="40.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="13" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>36</v>
+        <v>14</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D4" s="14" t="s">
-        <v>32</v>
+        <v>9</v>
       </c>
       <c r="E4" s="13" t="s">
         <v>11</v>
       </c>
       <c r="F4" s="13" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="G4" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="H4" s="17" t="s">
-        <v>29</v>
+        <v>16</v>
+      </c>
+      <c r="H4" s="16" t="s">
+        <v>26</v>
       </c>
       <c r="Q4" s="2"/>
     </row>
     <row r="5" spans="1:17" ht="46.5" x14ac:dyDescent="0.45">
       <c r="A5" s="13" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D5" s="14" t="s">
         <v>32</v>
@@ -923,21 +942,23 @@
       <c r="E5" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="13"/>
+      <c r="F5" s="13" t="s">
+        <v>37</v>
+      </c>
       <c r="G5" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="H5" s="18" t="s">
-        <v>9</v>
+        <v>38</v>
+      </c>
+      <c r="H5" s="17" t="s">
+        <v>29</v>
       </c>
       <c r="Q5" s="2"/>
     </row>
-    <row r="6" spans="1:17" ht="58.15" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:17" ht="46.5" x14ac:dyDescent="0.45">
       <c r="A6" s="13" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C6" s="14" t="s">
         <v>10</v>
@@ -948,56 +969,54 @@
       <c r="E6" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="13" t="s">
-        <v>44</v>
-      </c>
+      <c r="F6" s="13"/>
       <c r="G6" s="13" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="H6" s="18" t="s">
         <v>9</v>
       </c>
       <c r="Q6" s="2"/>
     </row>
-    <row r="7" spans="1:17" ht="23.25" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:17" ht="58.15" x14ac:dyDescent="0.45">
       <c r="A7" s="13" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C7" s="14" t="s">
         <v>10</v>
       </c>
       <c r="D7" s="14" t="s">
-        <v>10</v>
+        <v>32</v>
       </c>
       <c r="E7" s="13" t="s">
         <v>11</v>
       </c>
       <c r="F7" s="13" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="G7" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="H7" s="19" t="s">
-        <v>10</v>
+        <v>45</v>
+      </c>
+      <c r="H7" s="18" t="s">
+        <v>9</v>
       </c>
       <c r="Q7" s="2"/>
     </row>
-    <row r="8" spans="1:17" ht="24" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:17" ht="23.25" x14ac:dyDescent="0.45">
       <c r="A8" s="13" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C8" s="14" t="s">
         <v>10</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E8" s="13" t="s">
         <v>11</v>
@@ -1005,44 +1024,62 @@
       <c r="F8" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="G8" s="13"/>
-      <c r="H8" s="20" t="s">
+      <c r="G8" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="H8" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q8" s="2"/>
+    </row>
+    <row r="9" spans="1:17" ht="24" x14ac:dyDescent="0.45">
+      <c r="A9" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="G9" s="13"/>
+      <c r="H9" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="Q8" s="2"/>
-    </row>
-    <row r="9" spans="1:17" ht="23.25" x14ac:dyDescent="0.45">
-      <c r="A9" s="13" t="s">
+      <c r="Q9" s="2"/>
+    </row>
+    <row r="10" spans="1:17" ht="23.25" x14ac:dyDescent="0.45">
+      <c r="A10" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="B9" s="21" t="s">
+      <c r="B10" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="C9" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="D9" s="22" t="s">
+      <c r="C10" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="E9" s="21" t="s">
+      <c r="E10" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="F9" s="21"/>
-      <c r="G9" s="21" t="s">
+      <c r="F10" s="21"/>
+      <c r="G10" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="H9" s="18" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
+      <c r="H10" s="18" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.45">
       <c r="B11" s="4"/>
@@ -1054,17 +1091,18 @@
       <c r="H11" s="4"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A12" s="3" t="s">
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A13" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
@@ -1072,52 +1110,40 @@
       <c r="F13" s="3"/>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A14" s="6"/>
-      <c r="B14" s="6" t="s">
+      <c r="A14" s="3"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A15" s="6"/>
+      <c r="B15" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C15" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D14" s="6" t="s">
+      <c r="D15" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E14" s="6" t="s">
+      <c r="E15" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="F14" s="6" t="s">
+      <c r="F15" s="6" t="s">
         <v>22</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A15" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D15" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="E15" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="F15" s="9" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A16" s="6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B16" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C16" s="8" t="s">
-        <v>26</v>
+      <c r="C16" s="7" t="s">
+        <v>10</v>
       </c>
       <c r="D16" s="8" t="s">
         <v>24</v>
@@ -1125,13 +1151,13 @@
       <c r="E16" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="F16" s="10" t="s">
-        <v>27</v>
+      <c r="F16" s="9" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A17" s="6" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B17" s="7" t="s">
         <v>10</v>
@@ -1139,11 +1165,11 @@
       <c r="C17" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="D17" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E17" s="10" t="s">
-        <v>29</v>
+      <c r="D17" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="E17" s="9" t="s">
+        <v>9</v>
       </c>
       <c r="F17" s="10" t="s">
         <v>27</v>
@@ -1151,54 +1177,74 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A18" s="6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B18" s="7" t="s">
         <v>10</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D18" s="9" t="s">
         <v>9</v>
       </c>
       <c r="E18" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="F18" s="11" t="s">
-        <v>32</v>
+        <v>29</v>
+      </c>
+      <c r="F18" s="10" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A19" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="B19" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C19" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C19" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="D19" s="10" t="s">
+      <c r="D19" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E19" s="10" t="s">
         <v>31</v>
-      </c>
-      <c r="E19" s="11" t="s">
-        <v>32</v>
       </c>
       <c r="F19" s="11" t="s">
         <v>32</v>
       </c>
     </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A20" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="E20" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="F20" s="11" t="s">
+        <v>32</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="C2:D9">
-    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="Medium">
-      <formula>NOT(ISERROR(SEARCH("Medium",C2)))</formula>
+  <conditionalFormatting sqref="C3:D10">
+    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="High">
+      <formula>NOT(ISERROR(SEARCH("High",C3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="Low">
-      <formula>NOT(ISERROR(SEARCH("Low",C2)))</formula>
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="Low">
+      <formula>NOT(ISERROR(SEARCH("Low",C3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="High">
-      <formula>NOT(ISERROR(SEARCH("High",C2)))</formula>
+    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="Medium">
+      <formula>NOT(ISERROR(SEARCH("Medium",C3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>